<commit_message>
modified for Selenium Grid
</commit_message>
<xml_diff>
--- a/citeis-auto/inputs/TestData.xlsx
+++ b/citeis-auto/inputs/TestData.xlsx
@@ -24,13 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
-  <si>
-    <t>Execute</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>ITERATION</t>
   </si>
@@ -59,32 +53,15 @@
     <t>2</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>FIREFOX</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -133,9 +110,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
@@ -419,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:I1048576"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,92 +407,48 @@
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>0</v>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added execute column in testdata.xlsx
</commit_message>
<xml_diff>
--- a/citeis-auto/inputs/TestData.xlsx
+++ b/citeis-auto/inputs/TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pponguru\git\CITEIS\citeis-auto\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CITEIS_Automation\citeis-auto\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>ITERATION</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>FIREFOX</t>
+  </si>
+  <si>
+    <t>EXECUTE</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -110,11 +116,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -409,7 +416,7 @@
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -422,8 +429,11 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -436,8 +446,11 @@
       <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="E2" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -449,6 +462,9 @@
       </c>
       <c r="D3" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>